<commit_message>
Impleted the Point struct into the easing functions instead of using floats only
</commit_message>
<xml_diff>
--- a/EaseTypes.xlsx
+++ b/EaseTypes.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8E2633-A37D-4244-BA5A-846DB6F5A970}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A41F760-D0AD-4136-ABE7-35D91E9C18B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
   <si>
     <t>In</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>sqrt(2x-x^2)</t>
+  </si>
+  <si>
+    <t>Scaling a function will require you to divide the x values by the y scale, and to multiple the result of a function by the x scale</t>
   </si>
 </sst>
 </file>
@@ -574,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,6 +796,11 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>